<commit_message>
SHG pre test migr
</commit_message>
<xml_diff>
--- a/XLS Data/SHG.xlsx
+++ b/XLS Data/SHG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\eclipse-workspace\LokOSMain\XLS Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66566733-55E8-442D-9353-54683DDE873F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E978FD19-50EE-4E58-B1F1-5452545C032C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5943E96-0337-46EC-8631-731C3FE0A3A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5943E96-0337-46EC-8631-731C3FE0A3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,8 @@
 7) Cutoff Update(Do not use)
 8) Regular New
 9) Regular Update(Do not use)
-</t>
+10) &lt;00&gt;,&lt;00&gt;,... Migration
+ -&gt;Works on migrated data.</t>
         </r>
       </text>
     </comment>
@@ -247,8 +248,8 @@
 2) &lt;00&gt;,&lt;00&gt;,... Update
  -&gt;Should be ascending order
  -&gt;'Update can be changed to any message without space.
-3)&lt;00&gt;,&lt;00&gt;,... Check
- -&gt;Negetive Testing</t>
+3)&lt;00&gt;,&lt;00&gt;,... Check -&gt;Negetive Testing
+4) &lt;00&gt;,&lt;00&gt;,... Migration -&gt;Works on migrated data.</t>
         </r>
       </text>
     </comment>
@@ -353,7 +354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="554">
   <si>
     <t>App</t>
   </si>
@@ -1921,34 +1922,100 @@
     <t>Rahul:9455120510</t>
   </si>
   <si>
+    <t>#40256541474</t>
+  </si>
+  <si>
+    <t>#40256541476</t>
+  </si>
+  <si>
+    <t>#40256541478</t>
+  </si>
+  <si>
+    <t>20_04_2022</t>
+  </si>
+  <si>
+    <t>Aadhaar</t>
+  </si>
+  <si>
+    <t>GUJARAT TEST SHG</t>
+  </si>
+  <si>
+    <t>ALHADPURA</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>GJ_GJBK</t>
+  </si>
+  <si>
+    <t>19 Mobile Number</t>
+  </si>
+  <si>
+    <t>20 Address</t>
+  </si>
+  <si>
+    <t>21 Bank</t>
+  </si>
+  <si>
+    <t>22 President</t>
+  </si>
+  <si>
+    <t>23 Tresurar</t>
+  </si>
+  <si>
+    <t>24 Secretary</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Do Not Add</t>
+  </si>
+  <si>
     <t>Submit</t>
   </si>
   <si>
-    <t>#40256541474</t>
-  </si>
-  <si>
-    <t>#40256541476</t>
-  </si>
-  <si>
-    <t>#40256541478</t>
-  </si>
-  <si>
-    <t>20_04_2022</t>
-  </si>
-  <si>
-    <t>Aadhaar</t>
-  </si>
-  <si>
-    <t>GUJARAT TEST SHG</t>
-  </si>
-  <si>
-    <t>ALHADPURA</t>
-  </si>
-  <si>
-    <t>Gujarat</t>
-  </si>
-  <si>
-    <t>GJ_GJBK</t>
+    <t>40256541490</t>
+  </si>
+  <si>
+    <t>40256541495</t>
+  </si>
+  <si>
+    <t>110049</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>9455885271</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>BHADSON</t>
+  </si>
+  <si>
+    <t>HARYANA TEST SHG</t>
+  </si>
+  <si>
+    <t>40256541494</t>
+  </si>
+  <si>
+    <t>40256541493</t>
+  </si>
+  <si>
+    <t>40256541491</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -2481,7 +2548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2730,13 +2797,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3056,7 +3125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAFDE49-6EC4-411F-AEDE-4DE32D140FEF}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3093,7 +3162,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="87" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C2" t="s">
         <v>223</v>
@@ -3102,7 +3171,7 @@
         <v>224</v>
       </c>
       <c r="E2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>225</v>
@@ -3125,10 +3194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC1CF2F-DF31-4E4A-8DA8-3780D013A601}">
-  <dimension ref="A1:BI3"/>
+  <dimension ref="A1:BO15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="14.4"/>
@@ -3136,10 +3205,11 @@
     <col min="1" max="1" width="6.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.21875" style="1"/>
     <col min="3" max="3" width="20.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="15.21875" style="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="15.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="8" customFormat="1" ht="84" customHeight="1" thickBot="1">
+    <row r="1" spans="1:67" s="8" customFormat="1" ht="84" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3323,8 +3393,26 @@
       <c r="BI1" s="7" t="s">
         <v>66</v>
       </c>
+      <c r="BJ1" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="BK1" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="BL1" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="BM1" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="BN1" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="BO1" s="8" t="s">
+        <v>536</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" ht="28.8">
+    <row r="2" spans="1:67" ht="28.8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3335,13 +3423,13 @@
         <v>514</v>
       </c>
       <c r="D2" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="E2" t="s">
         <v>528</v>
       </c>
-      <c r="E2" t="s">
-        <v>529</v>
-      </c>
       <c r="F2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -3462,7 +3550,7 @@
         <v>516</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="BB2" s="1" t="s">
         <v>238</v>
@@ -3471,7 +3559,7 @@
         <v>517</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="BE2" s="1" t="s">
         <v>238</v>
@@ -3480,18 +3568,1498 @@
         <v>518</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="BH2" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="BJ2" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>537</v>
+      </c>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:67" ht="28.8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>522</v>
+      <c r="B3" t="s">
+        <v>513</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="E3" t="s">
+        <v>528</v>
+      </c>
+      <c r="F3" t="s">
+        <v>528</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U3" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>14</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>110049</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AX3"/>
+      <c r="AY3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO3" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67" ht="28.8">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>513</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="E4" t="s">
+        <v>528</v>
+      </c>
+      <c r="F4" t="s">
+        <v>528</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="M4" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U4" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>14</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>110049</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AX4"/>
+      <c r="AY4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC4" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD4" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF4" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG4" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK4" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL4" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM4" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN4" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO4" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" ht="28.8">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>513</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="E5" t="s">
+        <v>528</v>
+      </c>
+      <c r="F5" t="s">
+        <v>528</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="M5" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U5" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>14</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>110049</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT5" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AX5"/>
+      <c r="AY5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ5" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC5" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD5" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF5" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG5" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH5" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ5" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK5" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL5" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="BM5" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN5" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO5" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:67" ht="28.8">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>513</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>527</v>
+      </c>
+      <c r="E6" t="s">
+        <v>528</v>
+      </c>
+      <c r="F6" t="s">
+        <v>528</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L6" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="M6" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="U6" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>14</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>110049</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AX6"/>
+      <c r="AY6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ6" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC6" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD6" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF6" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG6" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH6" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ6" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK6" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL6" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM6" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="BN6" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="BO6" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67" s="59" customFormat="1">
+      <c r="B7" s="88" t="s">
+        <v>539</v>
+      </c>
+      <c r="D7" s="89"/>
+      <c r="G7" s="88"/>
+      <c r="AX7" s="88"/>
+    </row>
+    <row r="8" spans="1:67" s="59" customFormat="1" ht="28.8">
+      <c r="A8" s="59">
+        <v>2</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>513</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>514</v>
+      </c>
+      <c r="D8" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>553</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="J8" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="K8" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="M8" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="N8" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="O8" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="P8" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q8" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="S8" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="U8" s="59" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y8" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z8" s="59" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA8" s="59" t="s">
+        <v>545</v>
+      </c>
+      <c r="AB8" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC8" s="59" t="s">
+        <v>507</v>
+      </c>
+      <c r="AD8" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE8" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF8" s="59" t="s">
+        <v>544</v>
+      </c>
+      <c r="AG8" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH8" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI8" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ8" s="59" t="s">
+        <v>543</v>
+      </c>
+      <c r="AL8" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM8" s="59" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN8" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO8" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP8" s="59" t="s">
+        <v>542</v>
+      </c>
+      <c r="AQ8" s="59" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR8" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS8" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT8" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU8" s="59" t="s">
+        <v>552</v>
+      </c>
+      <c r="AV8" s="59" t="s">
+        <v>540</v>
+      </c>
+      <c r="AW8" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="AY8" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ8" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA8" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB8" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC8" s="59" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD8" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE8" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF8" s="59" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG8" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH8" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ8" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK8" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL8" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM8" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN8" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO8" s="59" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:67" s="59" customFormat="1">
+      <c r="B9" s="59" t="s">
+        <v>539</v>
+      </c>
+      <c r="D9" s="89"/>
+      <c r="G9" s="88"/>
+    </row>
+    <row r="10" spans="1:67" s="59" customFormat="1" ht="28.8">
+      <c r="A10" s="59">
+        <v>3</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>513</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>514</v>
+      </c>
+      <c r="D10" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="E10" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="G10" s="88" t="s">
+        <v>288</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="K10" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="L10" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="M10" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="N10" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="O10" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="P10" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q10" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="S10" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="U10" s="59" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y10" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z10" s="59" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA10" s="59" t="s">
+        <v>545</v>
+      </c>
+      <c r="AB10" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC10" s="59" t="s">
+        <v>507</v>
+      </c>
+      <c r="AD10" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE10" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF10" s="59" t="s">
+        <v>544</v>
+      </c>
+      <c r="AG10" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH10" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI10" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ10" s="59" t="s">
+        <v>543</v>
+      </c>
+      <c r="AL10" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM10" s="59" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN10" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO10" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP10" s="59" t="s">
+        <v>542</v>
+      </c>
+      <c r="AQ10" s="59" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR10" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS10" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT10" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU10" s="59" t="s">
+        <v>551</v>
+      </c>
+      <c r="AV10" s="59" t="s">
+        <v>540</v>
+      </c>
+      <c r="AW10" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="AY10" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ10" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA10" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB10" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC10" s="59" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD10" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE10" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF10" s="59" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG10" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH10" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ10" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK10" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL10" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM10" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN10" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO10" s="59" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:67" s="59" customFormat="1">
+      <c r="B11" s="59" t="s">
+        <v>539</v>
+      </c>
+      <c r="D11" s="89"/>
+      <c r="G11" s="88"/>
+    </row>
+    <row r="12" spans="1:67" s="59" customFormat="1" ht="28.8">
+      <c r="A12" s="59">
+        <v>4</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>513</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>514</v>
+      </c>
+      <c r="D12" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="G12" s="88" t="s">
+        <v>547</v>
+      </c>
+      <c r="H12" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="I12" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="J12" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="L12" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="M12" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="N12" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="O12" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="P12" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q12" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="S12" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="U12" s="59" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y12" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z12" s="59" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA12" s="59" t="s">
+        <v>545</v>
+      </c>
+      <c r="AB12" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC12" s="59" t="s">
+        <v>507</v>
+      </c>
+      <c r="AD12" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE12" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF12" s="59" t="s">
+        <v>544</v>
+      </c>
+      <c r="AG12" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH12" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI12" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ12" s="59" t="s">
+        <v>543</v>
+      </c>
+      <c r="AL12" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM12" s="59" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN12" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO12" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP12" s="59" t="s">
+        <v>542</v>
+      </c>
+      <c r="AQ12" s="59" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR12" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS12" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT12" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU12" s="59" t="s">
+        <v>550</v>
+      </c>
+      <c r="AV12" s="59" t="s">
+        <v>540</v>
+      </c>
+      <c r="AW12" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="AY12" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ12" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA12" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB12" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC12" s="59" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD12" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE12" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF12" s="59" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG12" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH12" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ12" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK12" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL12" s="59" t="s">
+        <v>538</v>
+      </c>
+      <c r="BM12" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BN12" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BO12" s="59" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:67" s="59" customFormat="1">
+      <c r="B13" s="59" t="s">
+        <v>539</v>
+      </c>
+      <c r="D13" s="89"/>
+      <c r="G13" s="88"/>
+    </row>
+    <row r="14" spans="1:67" s="59" customFormat="1" ht="28.8">
+      <c r="A14" s="59">
+        <v>5</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>513</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>514</v>
+      </c>
+      <c r="D14" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>548</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>547</v>
+      </c>
+      <c r="H14" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="I14" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="J14" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="K14" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="L14" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="M14" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="N14" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="O14" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="P14" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q14" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="S14" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="U14" s="59" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y14" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z14" s="59" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA14" s="59" t="s">
+        <v>545</v>
+      </c>
+      <c r="AB14" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC14" s="59" t="s">
+        <v>507</v>
+      </c>
+      <c r="AD14" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE14" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF14" s="59" t="s">
+        <v>544</v>
+      </c>
+      <c r="AG14" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH14" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI14" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ14" s="59" t="s">
+        <v>543</v>
+      </c>
+      <c r="AL14" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="AM14" s="59" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN14" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO14" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP14" s="59" t="s">
+        <v>542</v>
+      </c>
+      <c r="AQ14" s="59" t="s">
+        <v>515</v>
+      </c>
+      <c r="AR14" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS14" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT14" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU14" s="59" t="s">
+        <v>541</v>
+      </c>
+      <c r="AV14" s="59" t="s">
+        <v>540</v>
+      </c>
+      <c r="AW14" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="AY14" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ14" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="BA14" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BB14" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC14" s="59" t="s">
+        <v>517</v>
+      </c>
+      <c r="BD14" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE14" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF14" s="59" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG14" s="59" t="s">
+        <v>525</v>
+      </c>
+      <c r="BH14" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="BJ14" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BK14" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BL14" s="59" t="s">
+        <v>537</v>
+      </c>
+      <c r="BM14" s="59" t="s">
+        <v>538</v>
+      </c>
+      <c r="BN14" s="59" t="s">
+        <v>538</v>
+      </c>
+      <c r="BO14" s="59" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:67" s="59" customFormat="1">
+      <c r="B15" s="59" t="s">
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +5074,7 @@
   <dimension ref="A1:BH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="48.6" customHeight="1"/>
@@ -3703,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>254</v>
@@ -3832,7 +5400,7 @@
         <v>238</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>364</v>
@@ -3867,7 +5435,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>254</v>
@@ -3984,7 +5552,7 @@
         <v>238</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AW3" s="1" t="s">
         <v>364</v>
@@ -4019,7 +5587,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>254</v>
@@ -4136,10 +5704,10 @@
         <v>362</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>385</v>
@@ -4148,7 +5716,7 @@
         <v>238</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AW4" s="1" t="s">
         <v>364</v>
@@ -4183,7 +5751,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>254</v>
@@ -4288,10 +5856,10 @@
         <v>362</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AS5" s="1" t="s">
         <v>392</v>
@@ -4300,7 +5868,7 @@
         <v>238</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AW5" s="1" t="s">
         <v>364</v>
@@ -4335,7 +5903,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>254</v>
@@ -4452,10 +6020,10 @@
         <v>362</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>399</v>
@@ -4464,7 +6032,7 @@
         <v>238</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AW6" s="1" t="s">
         <v>364</v>
@@ -5099,172 +6667,172 @@
       <c r="E1" s="85"/>
       <c r="F1" s="85"/>
       <c r="G1" s="85"/>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="90" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="90"/>
-      <c r="J1" s="88" t="s">
+      <c r="I1" s="91"/>
+      <c r="J1" s="90" t="s">
         <v>293</v>
       </c>
-      <c r="K1" s="89"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="88" t="s">
+      <c r="K1" s="92"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="N1" s="89"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="88" t="s">
+      <c r="N1" s="92"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="90" t="s">
         <v>295</v>
       </c>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="90"/>
-      <c r="AA1" s="88" t="s">
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="90" t="s">
         <v>296</v>
       </c>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89"/>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="89"/>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="90"/>
-      <c r="AL1" s="88" t="s">
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="92"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="90" t="s">
         <v>297</v>
       </c>
-      <c r="AM1" s="89"/>
-      <c r="AN1" s="89"/>
-      <c r="AO1" s="89"/>
-      <c r="AP1" s="89"/>
-      <c r="AQ1" s="89"/>
-      <c r="AR1" s="89"/>
-      <c r="AS1" s="89"/>
-      <c r="AT1" s="89"/>
-      <c r="AU1" s="89"/>
-      <c r="AV1" s="89"/>
-      <c r="AW1" s="89"/>
-      <c r="AX1" s="89"/>
-      <c r="AY1" s="89"/>
-      <c r="AZ1" s="90"/>
-      <c r="BA1" s="88" t="s">
+      <c r="AM1" s="92"/>
+      <c r="AN1" s="92"/>
+      <c r="AO1" s="92"/>
+      <c r="AP1" s="92"/>
+      <c r="AQ1" s="92"/>
+      <c r="AR1" s="92"/>
+      <c r="AS1" s="92"/>
+      <c r="AT1" s="92"/>
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="92"/>
+      <c r="AW1" s="92"/>
+      <c r="AX1" s="92"/>
+      <c r="AY1" s="92"/>
+      <c r="AZ1" s="91"/>
+      <c r="BA1" s="90" t="s">
         <v>298</v>
       </c>
-      <c r="BB1" s="89"/>
-      <c r="BC1" s="89"/>
-      <c r="BD1" s="89"/>
-      <c r="BE1" s="89"/>
-      <c r="BF1" s="89"/>
-      <c r="BG1" s="89"/>
-      <c r="BH1" s="89"/>
-      <c r="BI1" s="89"/>
-      <c r="BJ1" s="89"/>
-      <c r="BK1" s="89"/>
-      <c r="BL1" s="89"/>
-      <c r="BM1" s="89"/>
-      <c r="BN1" s="89"/>
-      <c r="BO1" s="89"/>
-      <c r="BP1" s="89"/>
-      <c r="BQ1" s="89"/>
-      <c r="BR1" s="89"/>
-      <c r="BS1" s="89"/>
-      <c r="BT1" s="89"/>
-      <c r="BU1" s="90"/>
-      <c r="BV1" s="88" t="s">
+      <c r="BB1" s="92"/>
+      <c r="BC1" s="92"/>
+      <c r="BD1" s="92"/>
+      <c r="BE1" s="92"/>
+      <c r="BF1" s="92"/>
+      <c r="BG1" s="92"/>
+      <c r="BH1" s="92"/>
+      <c r="BI1" s="92"/>
+      <c r="BJ1" s="92"/>
+      <c r="BK1" s="92"/>
+      <c r="BL1" s="92"/>
+      <c r="BM1" s="92"/>
+      <c r="BN1" s="92"/>
+      <c r="BO1" s="92"/>
+      <c r="BP1" s="92"/>
+      <c r="BQ1" s="92"/>
+      <c r="BR1" s="92"/>
+      <c r="BS1" s="92"/>
+      <c r="BT1" s="92"/>
+      <c r="BU1" s="91"/>
+      <c r="BV1" s="90" t="s">
         <v>299</v>
       </c>
-      <c r="BW1" s="89"/>
-      <c r="BX1" s="90"/>
-      <c r="BY1" s="88" t="s">
+      <c r="BW1" s="92"/>
+      <c r="BX1" s="91"/>
+      <c r="BY1" s="90" t="s">
         <v>300</v>
       </c>
-      <c r="BZ1" s="89"/>
-      <c r="CA1" s="89"/>
-      <c r="CB1" s="89"/>
-      <c r="CC1" s="89"/>
-      <c r="CD1" s="89"/>
-      <c r="CE1" s="89"/>
-      <c r="CF1" s="89"/>
-      <c r="CG1" s="89"/>
-      <c r="CH1" s="89"/>
-      <c r="CI1" s="89"/>
-      <c r="CJ1" s="89"/>
-      <c r="CK1" s="90"/>
-      <c r="CL1" s="88" t="s">
+      <c r="BZ1" s="92"/>
+      <c r="CA1" s="92"/>
+      <c r="CB1" s="92"/>
+      <c r="CC1" s="92"/>
+      <c r="CD1" s="92"/>
+      <c r="CE1" s="92"/>
+      <c r="CF1" s="92"/>
+      <c r="CG1" s="92"/>
+      <c r="CH1" s="92"/>
+      <c r="CI1" s="92"/>
+      <c r="CJ1" s="92"/>
+      <c r="CK1" s="91"/>
+      <c r="CL1" s="90" t="s">
         <v>301</v>
       </c>
-      <c r="CM1" s="89"/>
-      <c r="CN1" s="89"/>
-      <c r="CO1" s="89"/>
-      <c r="CP1" s="89"/>
-      <c r="CQ1" s="89"/>
-      <c r="CR1" s="89"/>
-      <c r="CS1" s="89"/>
-      <c r="CT1" s="89"/>
-      <c r="CU1" s="89"/>
-      <c r="CV1" s="89"/>
-      <c r="CW1" s="89"/>
-      <c r="CX1" s="89"/>
-      <c r="CY1" s="89"/>
-      <c r="CZ1" s="89"/>
-      <c r="DA1" s="89"/>
-      <c r="DB1" s="89"/>
-      <c r="DC1" s="89"/>
-      <c r="DD1" s="89"/>
-      <c r="DE1" s="89"/>
-      <c r="DF1" s="89"/>
-      <c r="DG1" s="89"/>
-      <c r="DH1" s="89"/>
-      <c r="DI1" s="89"/>
-      <c r="DJ1" s="89"/>
-      <c r="DK1" s="89"/>
-      <c r="DL1" s="89"/>
-      <c r="DM1" s="89"/>
-      <c r="DN1" s="90"/>
-      <c r="DO1" s="88" t="s">
+      <c r="CM1" s="92"/>
+      <c r="CN1" s="92"/>
+      <c r="CO1" s="92"/>
+      <c r="CP1" s="92"/>
+      <c r="CQ1" s="92"/>
+      <c r="CR1" s="92"/>
+      <c r="CS1" s="92"/>
+      <c r="CT1" s="92"/>
+      <c r="CU1" s="92"/>
+      <c r="CV1" s="92"/>
+      <c r="CW1" s="92"/>
+      <c r="CX1" s="92"/>
+      <c r="CY1" s="92"/>
+      <c r="CZ1" s="92"/>
+      <c r="DA1" s="92"/>
+      <c r="DB1" s="92"/>
+      <c r="DC1" s="92"/>
+      <c r="DD1" s="92"/>
+      <c r="DE1" s="92"/>
+      <c r="DF1" s="92"/>
+      <c r="DG1" s="92"/>
+      <c r="DH1" s="92"/>
+      <c r="DI1" s="92"/>
+      <c r="DJ1" s="92"/>
+      <c r="DK1" s="92"/>
+      <c r="DL1" s="92"/>
+      <c r="DM1" s="92"/>
+      <c r="DN1" s="91"/>
+      <c r="DO1" s="90" t="s">
         <v>302</v>
       </c>
-      <c r="DP1" s="89"/>
-      <c r="DQ1" s="89"/>
-      <c r="DR1" s="89"/>
-      <c r="DS1" s="89"/>
-      <c r="DT1" s="89"/>
-      <c r="DU1" s="89"/>
-      <c r="DV1" s="89"/>
-      <c r="DW1" s="89"/>
-      <c r="DX1" s="89"/>
-      <c r="DY1" s="89"/>
-      <c r="DZ1" s="89"/>
-      <c r="EA1" s="90"/>
-      <c r="EB1" s="88" t="s">
+      <c r="DP1" s="92"/>
+      <c r="DQ1" s="92"/>
+      <c r="DR1" s="92"/>
+      <c r="DS1" s="92"/>
+      <c r="DT1" s="92"/>
+      <c r="DU1" s="92"/>
+      <c r="DV1" s="92"/>
+      <c r="DW1" s="92"/>
+      <c r="DX1" s="92"/>
+      <c r="DY1" s="92"/>
+      <c r="DZ1" s="92"/>
+      <c r="EA1" s="91"/>
+      <c r="EB1" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="EC1" s="89"/>
-      <c r="ED1" s="90"/>
-      <c r="EE1" s="88" t="s">
+      <c r="EC1" s="92"/>
+      <c r="ED1" s="91"/>
+      <c r="EE1" s="90" t="s">
         <v>303</v>
       </c>
-      <c r="EF1" s="89"/>
-      <c r="EG1" s="89"/>
-      <c r="EH1" s="89"/>
-      <c r="EI1" s="89"/>
-      <c r="EJ1" s="89"/>
-      <c r="EK1" s="89"/>
-      <c r="EL1" s="89"/>
-      <c r="EM1" s="89"/>
-      <c r="EN1" s="89"/>
-      <c r="EO1" s="89"/>
-      <c r="EP1" s="89"/>
-      <c r="EQ1" s="90"/>
+      <c r="EF1" s="92"/>
+      <c r="EG1" s="92"/>
+      <c r="EH1" s="92"/>
+      <c r="EI1" s="92"/>
+      <c r="EJ1" s="92"/>
+      <c r="EK1" s="92"/>
+      <c r="EL1" s="92"/>
+      <c r="EM1" s="92"/>
+      <c r="EN1" s="92"/>
+      <c r="EO1" s="92"/>
+      <c r="EP1" s="92"/>
+      <c r="EQ1" s="91"/>
     </row>
     <row r="2" spans="1:147" s="58" customFormat="1" ht="75.599999999999994" customHeight="1" thickBot="1">
       <c r="A2" s="47"/>
@@ -7091,11 +8659,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:Z1"/>
-    <mergeCell ref="CL1:DN1"/>
     <mergeCell ref="DO1:EA1"/>
     <mergeCell ref="EB1:ED1"/>
     <mergeCell ref="EE1:EQ1"/>
@@ -7104,6 +8667,11 @@
     <mergeCell ref="BA1:BU1"/>
     <mergeCell ref="BV1:BX1"/>
     <mergeCell ref="BY1:CK1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:Z1"/>
+    <mergeCell ref="CL1:DN1"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>